<commit_message>
fix registry_tutorial to register excel file.
</commit_message>
<xml_diff>
--- a/utils/questions.xlsx
+++ b/utils/questions.xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>